<commit_message>
libc and kernel compilation
</commit_message>
<xml_diff>
--- a/vee_16.xlsx
+++ b/vee_16.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13485" windowHeight="9255" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13485" windowHeight="9255" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ssh" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="lmbench_latency" sheetId="5" r:id="rId6"/>
     <sheet name="sshd_latency_new" sheetId="13" r:id="rId7"/>
     <sheet name="postmark" sheetId="14" r:id="rId8"/>
+    <sheet name="compilation" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3169" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3187" uniqueCount="255">
   <si>
     <t>nullSyscall</t>
   </si>
@@ -788,6 +789,15 @@
   <si>
     <t>svaKernel_opt_mmuChecks</t>
   </si>
+  <si>
+    <t>compiling libc: 10 rounds of execution</t>
+  </si>
+  <si>
+    <t>compiling kernel: 10 rounds of execution</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
 </sst>
 </file>
 
@@ -796,7 +806,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1015,6 +1025,13 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1387,7 +1404,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1533,6 +1550,7 @@
     </xf>
     <xf numFmtId="43" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1581,7 +1599,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -8380,11 +8401,11 @@
       <c r="D1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -8813,11 +8834,11 @@
       <c r="D20" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="91" t="s">
+      <c r="E20" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
@@ -9246,11 +9267,11 @@
       <c r="D39" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="91" t="s">
+      <c r="E39" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="91"/>
-      <c r="G39" s="91"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="92"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
@@ -9696,14 +9717,14 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="34"/>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="94" t="s">
+      <c r="C1" s="94"/>
+      <c r="D1" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="91"/>
+      <c r="E1" s="92"/>
     </row>
     <row r="2" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="34" t="s">
@@ -10030,14 +10051,14 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="34"/>
-      <c r="B21" s="92" t="s">
+      <c r="B21" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="93"/>
-      <c r="D21" s="94" t="s">
+      <c r="C21" s="94"/>
+      <c r="D21" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="91"/>
+      <c r="E21" s="92"/>
     </row>
     <row r="22" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="34" t="s">
@@ -10402,20 +10423,20 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="98" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
@@ -11013,20 +11034,20 @@
       </c>
     </row>
     <row r="19" spans="1:11" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="98" t="s">
+      <c r="C19" s="101"/>
+      <c r="D19" s="101"/>
+      <c r="E19" s="101"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="98"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="99"/>
+      <c r="K19" s="99"/>
     </row>
     <row r="20" spans="1:11" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="8" t="s">
@@ -11895,23 +11916,23 @@
       <c r="A15" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="102" t="s">
+      <c r="E15" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="102"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="102"/>
-      <c r="I15" s="102"/>
-      <c r="J15" s="102"/>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="102"/>
-      <c r="N15" s="102"/>
-      <c r="O15" s="102"/>
-      <c r="P15" s="102"/>
-      <c r="Q15" s="102"/>
-      <c r="R15" s="102"/>
-      <c r="S15" s="102"/>
+      <c r="F15" s="103"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="103"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="103"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="103"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="103"/>
+      <c r="O15" s="103"/>
+      <c r="P15" s="103"/>
+      <c r="Q15" s="103"/>
+      <c r="R15" s="103"/>
+      <c r="S15" s="103"/>
     </row>
     <row r="16" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -12749,23 +12770,23 @@
       <c r="A32" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="102" t="s">
+      <c r="E32" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="F32" s="102"/>
-      <c r="G32" s="102"/>
-      <c r="H32" s="102"/>
-      <c r="I32" s="102"/>
-      <c r="J32" s="102"/>
-      <c r="K32" s="102"/>
-      <c r="L32" s="102"/>
-      <c r="M32" s="102"/>
-      <c r="N32" s="102"/>
-      <c r="O32" s="102"/>
-      <c r="P32" s="102"/>
-      <c r="Q32" s="102"/>
-      <c r="R32" s="102"/>
-      <c r="S32" s="102"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="103"/>
+      <c r="I32" s="103"/>
+      <c r="J32" s="103"/>
+      <c r="K32" s="103"/>
+      <c r="L32" s="103"/>
+      <c r="M32" s="103"/>
+      <c r="N32" s="103"/>
+      <c r="O32" s="103"/>
+      <c r="P32" s="103"/>
+      <c r="Q32" s="103"/>
+      <c r="R32" s="103"/>
+      <c r="S32" s="103"/>
     </row>
     <row r="33" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
@@ -13775,23 +13796,23 @@
       <c r="A62" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="E62" s="102" t="s">
+      <c r="E62" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="F62" s="102"/>
-      <c r="G62" s="102"/>
-      <c r="H62" s="102"/>
-      <c r="I62" s="102"/>
-      <c r="J62" s="102"/>
-      <c r="K62" s="102"/>
-      <c r="L62" s="102"/>
-      <c r="M62" s="102"/>
-      <c r="N62" s="102"/>
-      <c r="O62" s="102"/>
-      <c r="P62" s="102"/>
-      <c r="Q62" s="102"/>
-      <c r="R62" s="102"/>
-      <c r="S62" s="102"/>
+      <c r="F62" s="103"/>
+      <c r="G62" s="103"/>
+      <c r="H62" s="103"/>
+      <c r="I62" s="103"/>
+      <c r="J62" s="103"/>
+      <c r="K62" s="103"/>
+      <c r="L62" s="103"/>
+      <c r="M62" s="103"/>
+      <c r="N62" s="103"/>
+      <c r="O62" s="103"/>
+      <c r="P62" s="103"/>
+      <c r="Q62" s="103"/>
+      <c r="R62" s="103"/>
+      <c r="S62" s="103"/>
     </row>
     <row r="63" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
@@ -14626,23 +14647,23 @@
       <c r="A79" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="E79" s="102" t="s">
+      <c r="E79" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="F79" s="102"/>
-      <c r="G79" s="102"/>
-      <c r="H79" s="102"/>
-      <c r="I79" s="102"/>
-      <c r="J79" s="102"/>
-      <c r="K79" s="102"/>
-      <c r="L79" s="102"/>
-      <c r="M79" s="102"/>
-      <c r="N79" s="102"/>
-      <c r="O79" s="102"/>
-      <c r="P79" s="102"/>
-      <c r="Q79" s="102"/>
-      <c r="R79" s="102"/>
-      <c r="S79" s="102"/>
+      <c r="F79" s="103"/>
+      <c r="G79" s="103"/>
+      <c r="H79" s="103"/>
+      <c r="I79" s="103"/>
+      <c r="J79" s="103"/>
+      <c r="K79" s="103"/>
+      <c r="L79" s="103"/>
+      <c r="M79" s="103"/>
+      <c r="N79" s="103"/>
+      <c r="O79" s="103"/>
+      <c r="P79" s="103"/>
+      <c r="Q79" s="103"/>
+      <c r="R79" s="103"/>
+      <c r="S79" s="103"/>
     </row>
     <row r="80" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
@@ -15839,23 +15860,23 @@
       <c r="A126" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="E126" s="102" t="s">
+      <c r="E126" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="F126" s="102"/>
-      <c r="G126" s="102"/>
-      <c r="H126" s="102"/>
-      <c r="I126" s="102"/>
-      <c r="J126" s="102"/>
-      <c r="K126" s="102"/>
-      <c r="L126" s="102"/>
-      <c r="M126" s="102"/>
-      <c r="N126" s="102"/>
-      <c r="O126" s="102"/>
-      <c r="P126" s="102"/>
-      <c r="Q126" s="102"/>
-      <c r="R126" s="102"/>
-      <c r="S126" s="102"/>
+      <c r="F126" s="103"/>
+      <c r="G126" s="103"/>
+      <c r="H126" s="103"/>
+      <c r="I126" s="103"/>
+      <c r="J126" s="103"/>
+      <c r="K126" s="103"/>
+      <c r="L126" s="103"/>
+      <c r="M126" s="103"/>
+      <c r="N126" s="103"/>
+      <c r="O126" s="103"/>
+      <c r="P126" s="103"/>
+      <c r="Q126" s="103"/>
+      <c r="R126" s="103"/>
+      <c r="S126" s="103"/>
     </row>
     <row r="127" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
@@ -16634,23 +16655,23 @@
       <c r="A141" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="E141" s="102" t="s">
+      <c r="E141" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="F141" s="102"/>
-      <c r="G141" s="102"/>
-      <c r="H141" s="102"/>
-      <c r="I141" s="102"/>
-      <c r="J141" s="102"/>
-      <c r="K141" s="102"/>
-      <c r="L141" s="102"/>
-      <c r="M141" s="102"/>
-      <c r="N141" s="102"/>
-      <c r="O141" s="102"/>
-      <c r="P141" s="102"/>
-      <c r="Q141" s="102"/>
-      <c r="R141" s="102"/>
-      <c r="S141" s="102"/>
+      <c r="F141" s="103"/>
+      <c r="G141" s="103"/>
+      <c r="H141" s="103"/>
+      <c r="I141" s="103"/>
+      <c r="J141" s="103"/>
+      <c r="K141" s="103"/>
+      <c r="L141" s="103"/>
+      <c r="M141" s="103"/>
+      <c r="N141" s="103"/>
+      <c r="O141" s="103"/>
+      <c r="P141" s="103"/>
+      <c r="Q141" s="103"/>
+      <c r="R141" s="103"/>
+      <c r="S141" s="103"/>
     </row>
     <row r="142" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
@@ -17768,23 +17789,23 @@
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
-      <c r="E167" s="103" t="s">
+      <c r="E167" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="F167" s="103"/>
-      <c r="G167" s="103"/>
-      <c r="H167" s="103"/>
-      <c r="I167" s="103"/>
-      <c r="J167" s="103"/>
-      <c r="K167" s="103"/>
-      <c r="L167" s="103"/>
-      <c r="M167" s="103"/>
-      <c r="N167" s="103"/>
-      <c r="O167" s="103"/>
-      <c r="P167" s="103"/>
-      <c r="Q167" s="103"/>
-      <c r="R167" s="103"/>
-      <c r="S167" s="103"/>
+      <c r="F167" s="104"/>
+      <c r="G167" s="104"/>
+      <c r="H167" s="104"/>
+      <c r="I167" s="104"/>
+      <c r="J167" s="104"/>
+      <c r="K167" s="104"/>
+      <c r="L167" s="104"/>
+      <c r="M167" s="104"/>
+      <c r="N167" s="104"/>
+      <c r="O167" s="104"/>
+      <c r="P167" s="104"/>
+      <c r="Q167" s="104"/>
+      <c r="R167" s="104"/>
+      <c r="S167" s="104"/>
     </row>
     <row r="168" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A168" s="1" t="s">
@@ -18328,23 +18349,23 @@
       <c r="A186" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="E186" s="102" t="s">
+      <c r="E186" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="F186" s="102"/>
-      <c r="G186" s="102"/>
-      <c r="H186" s="102"/>
-      <c r="I186" s="102"/>
-      <c r="J186" s="102"/>
-      <c r="K186" s="102"/>
-      <c r="L186" s="102"/>
-      <c r="M186" s="102"/>
-      <c r="N186" s="102"/>
-      <c r="O186" s="102"/>
-      <c r="P186" s="102"/>
-      <c r="Q186" s="102"/>
-      <c r="R186" s="102"/>
-      <c r="S186" s="102"/>
+      <c r="F186" s="103"/>
+      <c r="G186" s="103"/>
+      <c r="H186" s="103"/>
+      <c r="I186" s="103"/>
+      <c r="J186" s="103"/>
+      <c r="K186" s="103"/>
+      <c r="L186" s="103"/>
+      <c r="M186" s="103"/>
+      <c r="N186" s="103"/>
+      <c r="O186" s="103"/>
+      <c r="P186" s="103"/>
+      <c r="Q186" s="103"/>
+      <c r="R186" s="103"/>
+      <c r="S186" s="103"/>
     </row>
     <row r="187" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
@@ -18470,19 +18491,19 @@
       </c>
     </row>
     <row r="194" spans="1:4" s="83" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B194" s="102" t="s">
+      <c r="B194" s="103" t="s">
         <v>195</v>
       </c>
-      <c r="C194" s="102" t="s">
+      <c r="C194" s="103" t="s">
         <v>196</v>
       </c>
-      <c r="D194" s="102"/>
+      <c r="D194" s="103"/>
     </row>
     <row r="195" spans="1:4" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A195" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B195" s="102"/>
+      <c r="B195" s="103"/>
       <c r="C195" s="2" t="s">
         <v>185</v>
       </c>
@@ -18576,16 +18597,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B194:B195"/>
+    <mergeCell ref="C194:D194"/>
+    <mergeCell ref="E167:S167"/>
+    <mergeCell ref="E186:S186"/>
+    <mergeCell ref="E141:S141"/>
     <mergeCell ref="E15:S15"/>
     <mergeCell ref="E32:S32"/>
     <mergeCell ref="E62:S62"/>
     <mergeCell ref="E79:S79"/>
     <mergeCell ref="E126:S126"/>
-    <mergeCell ref="B194:B195"/>
-    <mergeCell ref="C194:D194"/>
-    <mergeCell ref="E167:S167"/>
-    <mergeCell ref="E186:S186"/>
-    <mergeCell ref="E141:S141"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18620,23 +18641,23 @@
       <c r="A1" s="79" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="105" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104" t="s">
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="104"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="44"/>
@@ -19269,11 +19290,11 @@
       <c r="A25" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="105" t="s">
+      <c r="C25" s="106" t="s">
         <v>185</v>
       </c>
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="106"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B26" s="40" t="s">
@@ -19496,14 +19517,14 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B40" s="106" t="s">
+      <c r="B40" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="C40" s="106"/>
-      <c r="D40" s="106" t="s">
+      <c r="C40" s="107"/>
+      <c r="D40" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="E40" s="106"/>
+      <c r="E40" s="107"/>
     </row>
     <row r="41" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B41" s="2" t="s">
@@ -19678,7 +19699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+    <sheetView topLeftCell="A98" workbookViewId="0">
       <selection activeCell="H107" sqref="H107"/>
     </sheetView>
   </sheetViews>
@@ -19709,23 +19730,23 @@
       <c r="A2" s="84" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="107" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
       <c r="I2" s="74"/>
-      <c r="J2" s="106" t="s">
+      <c r="J2" s="107" t="s">
         <v>178</v>
       </c>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="107"/>
     </row>
     <row r="3" spans="1:17" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -19880,14 +19901,14 @@
       <c r="C7" s="83"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="107" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
-      <c r="G8" s="106"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107"/>
+      <c r="G8" s="107"/>
     </row>
     <row r="9" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="83" t="s">
@@ -20168,23 +20189,23 @@
       <c r="A34" s="85" t="s">
         <v>205</v>
       </c>
-      <c r="E34" s="102" t="s">
+      <c r="E34" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="F34" s="102"/>
-      <c r="G34" s="102"/>
-      <c r="H34" s="102"/>
-      <c r="I34" s="102"/>
-      <c r="J34" s="102"/>
-      <c r="K34" s="102"/>
-      <c r="L34" s="102"/>
-      <c r="M34" s="102"/>
-      <c r="N34" s="102"/>
-      <c r="O34" s="102"/>
-      <c r="P34" s="102"/>
-      <c r="Q34" s="102"/>
-      <c r="R34" s="102"/>
-      <c r="S34" s="102"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="103"/>
+      <c r="H34" s="103"/>
+      <c r="I34" s="103"/>
+      <c r="J34" s="103"/>
+      <c r="K34" s="103"/>
+      <c r="L34" s="103"/>
+      <c r="M34" s="103"/>
+      <c r="N34" s="103"/>
+      <c r="O34" s="103"/>
+      <c r="P34" s="103"/>
+      <c r="Q34" s="103"/>
+      <c r="R34" s="103"/>
+      <c r="S34" s="103"/>
     </row>
     <row r="35" spans="1:19" s="83" customFormat="1" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A35" s="83" t="s">
@@ -22027,23 +22048,23 @@
       <c r="B70" s="83"/>
       <c r="C70" s="83"/>
       <c r="D70" s="83"/>
-      <c r="E70" s="102" t="s">
+      <c r="E70" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="F70" s="102"/>
-      <c r="G70" s="102"/>
-      <c r="H70" s="102"/>
-      <c r="I70" s="102"/>
-      <c r="J70" s="102"/>
-      <c r="K70" s="102"/>
-      <c r="L70" s="102"/>
-      <c r="M70" s="102"/>
-      <c r="N70" s="102"/>
-      <c r="O70" s="102"/>
-      <c r="P70" s="102"/>
-      <c r="Q70" s="102"/>
-      <c r="R70" s="102"/>
-      <c r="S70" s="102"/>
+      <c r="F70" s="103"/>
+      <c r="G70" s="103"/>
+      <c r="H70" s="103"/>
+      <c r="I70" s="103"/>
+      <c r="J70" s="103"/>
+      <c r="K70" s="103"/>
+      <c r="L70" s="103"/>
+      <c r="M70" s="103"/>
+      <c r="N70" s="103"/>
+      <c r="O70" s="103"/>
+      <c r="P70" s="103"/>
+      <c r="Q70" s="103"/>
+      <c r="R70" s="103"/>
+      <c r="S70" s="103"/>
     </row>
     <row r="71" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A71" s="83" t="s">
@@ -24293,7 +24314,7 @@
       </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A112" s="107" t="s">
+      <c r="A112" s="91" t="s">
         <v>136</v>
       </c>
       <c r="B112" s="1">
@@ -31650,4 +31671,207 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="22.73046875" customWidth="1"/>
+    <col min="3" max="3" width="18.1328125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="108" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="44.25" x14ac:dyDescent="0.65">
+      <c r="A2" s="109"/>
+      <c r="B2" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1">
+        <v>237607384207</v>
+      </c>
+      <c r="C3" s="1">
+        <v>109780857.443</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="1">
+        <v>260207926934</v>
+      </c>
+      <c r="C4" s="1">
+        <v>850451482.56900001</v>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/B3</f>
+        <v>1.0951171732411764</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="83" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="1">
+        <v>264787867362</v>
+      </c>
+      <c r="C5" s="1">
+        <v>149144238.44</v>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/B3</f>
+        <v>1.1143924177512967</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="83" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="1">
+        <v>281609621402</v>
+      </c>
+      <c r="C6" s="1">
+        <v>174845541.53799999</v>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/B3</f>
+        <v>1.1851888456322801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="83" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="1">
+        <v>286462916721</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1057512634.41</v>
+      </c>
+      <c r="D7" s="1">
+        <f>B7/B3</f>
+        <v>1.2056145379364043</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1">
+        <v>295055296920</v>
+      </c>
+      <c r="C8" s="1">
+        <v>141212480.92399999</v>
+      </c>
+      <c r="D8" s="1">
+        <f>B8/B3</f>
+        <v>1.241776630405359</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.65">
+      <c r="A11" s="108" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1864313933090</v>
+      </c>
+      <c r="C13" s="83">
+        <v>409164624.30299997</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1937143909450</v>
+      </c>
+      <c r="C14" s="83">
+        <v>463422522.74199998</v>
+      </c>
+      <c r="D14" s="1">
+        <f>B14/B13</f>
+        <v>1.0390652963899101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="83" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2043667226810</v>
+      </c>
+      <c r="C15" s="83">
+        <v>572298438.24899995</v>
+      </c>
+      <c r="D15" s="1">
+        <f>B15/B13</f>
+        <v>1.0962033756958152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2069036104130</v>
+      </c>
+      <c r="C16" s="83">
+        <v>375160414.21899998</v>
+      </c>
+      <c r="D16" s="1">
+        <f>B16/B13</f>
+        <v>1.1098109966386853</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
kernel option latency analysis
</commit_message>
<xml_diff>
--- a/vee_16.xlsx
+++ b/vee_16.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13485" windowHeight="9255" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13485" windowHeight="9255" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ssh" sheetId="4" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="postmark" sheetId="14" r:id="rId8"/>
     <sheet name="compilation" sheetId="15" r:id="rId9"/>
     <sheet name="summary-TLB-WP" sheetId="18" r:id="rId10"/>
+    <sheet name="kernel-op-latency" sheetId="21" r:id="rId11"/>
+    <sheet name="macrobench_wp" sheetId="20" r:id="rId12"/>
+    <sheet name="pap" sheetId="19" r:id="rId13"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4934" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5042" uniqueCount="378">
   <si>
     <t>nullSyscall</t>
   </si>
@@ -991,6 +994,183 @@
   <si>
     <t>svaKernel_nobatch (flush entire TLB without WP)</t>
   </si>
+  <si>
+    <t>time command output</t>
+  </si>
+  <si>
+    <t>postmark</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>with WP bit</t>
+  </si>
+  <si>
+    <t>without WP bit</t>
+  </si>
+  <si>
+    <t>null syscall</t>
+  </si>
+  <si>
+    <t>open/close</t>
+  </si>
+  <si>
+    <t>mmap</t>
+  </si>
+  <si>
+    <t>page fault</t>
+  </si>
+  <si>
+    <t>signal handler install</t>
+  </si>
+  <si>
+    <t>signal handler delivery</t>
+  </si>
+  <si>
+    <t>fork + exit</t>
+  </si>
+  <si>
+    <t>fork + exec</t>
+  </si>
+  <si>
+    <t>libc compilation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sshd </t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>With WP bit</t>
+  </si>
+  <si>
+    <t>Without WP bit</t>
+  </si>
+  <si>
+    <t>Overhead</t>
+  </si>
+  <si>
+    <t>SVA-OS batch-mode API</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>batch version with WP</t>
+  </si>
+  <si>
+    <t>sys</t>
+  </si>
+  <si>
+    <t>avg (second)</t>
+  </si>
+  <si>
+    <t>std (second)</t>
+  </si>
+  <si>
+    <t>unlink</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>write</t>
+  </si>
+  <si>
+    <t>lstat</t>
+  </si>
+  <si>
+    <t>fstat</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>lseek</t>
+  </si>
+  <si>
+    <t>execve</t>
+  </si>
+  <si>
+    <t>madvise</t>
+  </si>
+  <si>
+    <t>clock_gettime</t>
+  </si>
+  <si>
+    <t>sigprocmask</t>
+  </si>
+  <si>
+    <t>access</t>
+  </si>
+  <si>
+    <t>pread</t>
+  </si>
+  <si>
+    <t>munmap</t>
+  </si>
+  <si>
+    <t>readlink</t>
+  </si>
+  <si>
+    <t>issetugid</t>
+  </si>
+  <si>
+    <t>sysarch</t>
+  </si>
+  <si>
+    <t>ioctl</t>
+  </si>
+  <si>
+    <t>break</t>
+  </si>
+  <si>
+    <t>syscall</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>Postmark (aggregate results of 20 rounds)</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>svaKernel_no_instr</t>
+  </si>
+  <si>
+    <t>svaKernel_sfi</t>
+  </si>
+  <si>
+    <t>SVA-OS</t>
+  </si>
+  <si>
+    <t>CFI</t>
+  </si>
+  <si>
+    <t>SFI</t>
+  </si>
+  <si>
+    <t>Overhead(normalized to the baseline)</t>
+  </si>
+  <si>
+    <t>libc-compilation</t>
+  </si>
+  <si>
+    <t>SSHD ?</t>
+  </si>
 </sst>
 </file>
 
@@ -1424,7 +1604,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1557,6 +1737,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1604,7 +1804,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1793,6 +1993,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1845,6 +2056,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3306,6 +3520,307 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Overhead of</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> enabling/disabling WP bit</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pap!$D$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>overhead</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>pap!$A$14:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>postmark</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>libc compilation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sshd </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pap!$D$14:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0131653208722931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0476055693976161</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0537880198181984</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B908-45FE-AA66-282324042A69}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="554112280"/>
+        <c:axId val="554112608"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="554112280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554112608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="554112608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554112280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000" baseline="0"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3347,6 +3862,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4392,6 +4947,520 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4409,7 +5478,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4439,7 +5514,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4454,6 +5535,39 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656236" cy="6285453"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8617,10 +9731,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S158"/>
+  <dimension ref="A1:S165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E65" workbookViewId="0">
-      <selection activeCell="L65" sqref="L65:Q74"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8921,29 +10035,29 @@
     </row>
     <row r="27" spans="1:14" ht="61.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="7"/>
-      <c r="B27" s="125" t="s">
+      <c r="B27" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="125"/>
-      <c r="D27" s="125" t="s">
+      <c r="C27" s="130"/>
+      <c r="D27" s="130" t="s">
         <v>274</v>
       </c>
-      <c r="E27" s="125"/>
-      <c r="F27" s="125"/>
-      <c r="G27" s="125" t="s">
+      <c r="E27" s="130"/>
+      <c r="F27" s="130"/>
+      <c r="G27" s="130" t="s">
         <v>275</v>
       </c>
-      <c r="H27" s="125"/>
-      <c r="I27" s="125"/>
-      <c r="J27" s="124" t="s">
+      <c r="H27" s="130"/>
+      <c r="I27" s="130"/>
+      <c r="J27" s="129" t="s">
         <v>280</v>
       </c>
-      <c r="K27" s="124"/>
-      <c r="L27" s="124"/>
-      <c r="M27" s="124" t="s">
+      <c r="K27" s="129"/>
+      <c r="L27" s="129"/>
+      <c r="M27" s="129" t="s">
         <v>285</v>
       </c>
-      <c r="N27" s="124"/>
+      <c r="N27" s="129"/>
     </row>
     <row r="28" spans="1:14" ht="43.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="98"/>
@@ -9706,34 +10820,34 @@
     </row>
     <row r="65" spans="1:17" ht="55.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="7"/>
-      <c r="B65" s="125" t="s">
+      <c r="B65" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="C65" s="125"/>
-      <c r="D65" s="119" t="s">
+      <c r="C65" s="130"/>
+      <c r="D65" s="124" t="s">
         <v>280</v>
       </c>
-      <c r="E65" s="119"/>
-      <c r="F65" s="119"/>
-      <c r="G65" s="119" t="s">
+      <c r="E65" s="124"/>
+      <c r="F65" s="124"/>
+      <c r="G65" s="124" t="s">
         <v>292</v>
       </c>
-      <c r="H65" s="119"/>
-      <c r="I65" s="119"/>
-      <c r="J65" s="119" t="s">
+      <c r="H65" s="124"/>
+      <c r="I65" s="124"/>
+      <c r="J65" s="124" t="s">
         <v>285</v>
       </c>
-      <c r="K65" s="119"/>
-      <c r="L65" s="119" t="s">
+      <c r="K65" s="124"/>
+      <c r="L65" s="124" t="s">
         <v>312</v>
       </c>
-      <c r="M65" s="119"/>
-      <c r="N65" s="119"/>
-      <c r="O65" s="119" t="s">
+      <c r="M65" s="124"/>
+      <c r="N65" s="124"/>
+      <c r="O65" s="124" t="s">
         <v>318</v>
       </c>
-      <c r="P65" s="119"/>
-      <c r="Q65" s="119"/>
+      <c r="P65" s="124"/>
+      <c r="Q65" s="124"/>
     </row>
     <row r="66" spans="1:17" ht="43.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="98"/>
@@ -9829,7 +10943,7 @@
         <v>0.46169809356300001</v>
       </c>
       <c r="N67" s="1">
-        <f>L67/B67</f>
+        <f t="shared" ref="N67:N74" si="3">L67/B67</f>
         <v>1.0991099344063726</v>
       </c>
       <c r="O67" s="1">
@@ -9839,7 +10953,7 @@
         <v>0.59020417958500004</v>
       </c>
       <c r="Q67" s="1">
-        <f>O67/B67</f>
+        <f t="shared" ref="Q67:Q74" si="4">O67/B67</f>
         <v>1.0559082640700765</v>
       </c>
     </row>
@@ -9860,7 +10974,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="F68" s="1">
-        <f t="shared" ref="F68:F74" si="3">D68/B68</f>
+        <f t="shared" ref="F68:F74" si="5">D68/B68</f>
         <v>3.0301369863013701</v>
       </c>
       <c r="G68" s="1">
@@ -9870,7 +10984,7 @@
         <v>4.8989794855699998E-5</v>
       </c>
       <c r="I68" s="1">
-        <f t="shared" ref="I68:I74" si="4">G68/B68</f>
+        <f t="shared" ref="I68:I74" si="6">G68/B68</f>
         <v>3.0303860523038608</v>
       </c>
       <c r="J68" s="1">
@@ -9886,7 +11000,7 @@
         <v>4.8989794855699998E-5</v>
       </c>
       <c r="N68" s="1">
-        <f>L68/B68</f>
+        <f t="shared" si="3"/>
         <v>3.0094645080946454</v>
       </c>
       <c r="O68" s="1">
@@ -9896,7 +11010,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="Q68" s="1">
-        <f>O68/B68</f>
+        <f t="shared" si="4"/>
         <v>3.0093399750934</v>
       </c>
     </row>
@@ -9917,7 +11031,7 @@
         <v>1.35014814002E-3</v>
       </c>
       <c r="F69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.4437758781888608</v>
       </c>
       <c r="G69" s="1">
@@ -9927,7 +11041,7 @@
         <v>5.74696441611E-3</v>
       </c>
       <c r="I69" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.4682649926539333</v>
       </c>
       <c r="J69" s="1">
@@ -9943,7 +11057,7 @@
         <v>1.28534042183E-3</v>
       </c>
       <c r="N69" s="1">
-        <f>L69/B69</f>
+        <f t="shared" si="3"/>
         <v>2.4011419794310136</v>
       </c>
       <c r="O69" s="1">
@@ -9953,7 +11067,7 @@
         <v>8.8275081421699993E-3</v>
       </c>
       <c r="Q69" s="1">
-        <f>O69/B69</f>
+        <f t="shared" si="4"/>
         <v>2.4190530252437559</v>
       </c>
     </row>
@@ -9974,7 +11088,7 @@
         <v>0.17357511803299999</v>
       </c>
       <c r="F70" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.4494822842411859</v>
       </c>
       <c r="G70" s="1">
@@ -9984,7 +11098,7 @@
         <v>0.111077513926</v>
       </c>
       <c r="I70" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.3129635219631974</v>
       </c>
       <c r="J70" s="50">
@@ -10000,7 +11114,7 @@
         <v>0.11365445041900001</v>
       </c>
       <c r="N70" s="1">
-        <f>L70/B70</f>
+        <f t="shared" si="3"/>
         <v>3.9312255821771314</v>
       </c>
       <c r="O70" s="1">
@@ -10010,7 +11124,7 @@
         <v>0.73489522253200001</v>
       </c>
       <c r="Q70" s="1">
-        <f>O70/B70</f>
+        <f t="shared" si="4"/>
         <v>2.3703194217725145</v>
       </c>
     </row>
@@ -10031,7 +11145,7 @@
         <v>0.152933036326</v>
       </c>
       <c r="F71" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.4838303082195439</v>
       </c>
       <c r="G71" s="1">
@@ -10041,7 +11155,7 @@
         <v>6.02414807255E-2</v>
       </c>
       <c r="I71" s="50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.3356676853436191</v>
       </c>
       <c r="J71" s="50">
@@ -10057,7 +11171,7 @@
         <v>0.104613574645</v>
       </c>
       <c r="N71" s="1">
-        <f>L71/B71</f>
+        <f t="shared" si="3"/>
         <v>4.1097234149304382</v>
       </c>
       <c r="O71" s="1">
@@ -10067,7 +11181,7 @@
         <v>1.0695213774900001</v>
       </c>
       <c r="Q71" s="1">
-        <f>O71/B71</f>
+        <f t="shared" si="4"/>
         <v>2.4063798456192584</v>
       </c>
     </row>
@@ -10088,35 +11202,35 @@
         <v>2.22044604925E-16</v>
       </c>
       <c r="F72" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G72" s="1">
+        <v>1.048576</v>
+      </c>
+      <c r="H72" s="1">
+        <v>2.22044604925E-16</v>
+      </c>
+      <c r="I72" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J72" s="50">
+        <v>6628990.5999999996</v>
+      </c>
+      <c r="K72" s="50">
+        <v>1924148.9351600001</v>
+      </c>
+      <c r="L72" s="1">
+        <v>1.048576</v>
+      </c>
+      <c r="M72" s="1">
+        <v>2.22044604925E-16</v>
+      </c>
+      <c r="N72" s="1">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G72" s="1">
-        <v>1.048576</v>
-      </c>
-      <c r="H72" s="1">
-        <v>2.22044604925E-16</v>
-      </c>
-      <c r="I72" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J72" s="50">
-        <v>6628990.5999999996</v>
-      </c>
-      <c r="K72" s="50">
-        <v>1924148.9351600001</v>
-      </c>
-      <c r="L72" s="1">
-        <v>1.048576</v>
-      </c>
-      <c r="M72" s="1">
-        <v>2.22044604925E-16</v>
-      </c>
-      <c r="N72" s="1">
-        <f>L72/B72</f>
-        <v>1</v>
-      </c>
       <c r="O72" s="1">
         <v>1.048576</v>
       </c>
@@ -10124,7 +11238,7 @@
         <v>2.22044604925E-16</v>
       </c>
       <c r="Q72" s="1">
-        <f>O72/B72</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -10145,7 +11259,7 @@
         <v>2.8354893757500001E-4</v>
       </c>
       <c r="F73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.98819196186762004</v>
       </c>
       <c r="G73" s="1">
@@ -10155,7 +11269,7 @@
         <v>1.2621014222299999E-3</v>
       </c>
       <c r="I73" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.99042176723359698</v>
       </c>
       <c r="J73" s="1">
@@ -10171,7 +11285,7 @@
         <v>1.1634431657800001E-3</v>
       </c>
       <c r="N73" s="1">
-        <f>L73/B73</f>
+        <f t="shared" si="3"/>
         <v>0.98591701874119808</v>
       </c>
       <c r="O73" s="1">
@@ -10181,7 +11295,7 @@
         <v>8.8226980000399998E-4</v>
       </c>
       <c r="Q73" s="1">
-        <f>O73/B73</f>
+        <f t="shared" si="4"/>
         <v>0.98784891488823889</v>
       </c>
     </row>
@@ -10202,7 +11316,7 @@
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="F74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.4575798776342621</v>
       </c>
       <c r="G74" s="1">
@@ -10212,7 +11326,7 @@
         <v>5.5511151231299994E-17</v>
       </c>
       <c r="I74" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.4581917063222294</v>
       </c>
       <c r="J74" s="1">
@@ -10228,7 +11342,7 @@
         <v>4.4721359549999997E-5</v>
       </c>
       <c r="N74" s="1">
-        <f>L74/B74</f>
+        <f t="shared" si="3"/>
         <v>2.4473147518694764</v>
       </c>
       <c r="O74" s="1">
@@ -10238,7 +11352,7 @@
         <v>4.8989794855699998E-5</v>
       </c>
       <c r="Q74" s="1">
-        <f>O74/B74</f>
+        <f t="shared" si="4"/>
         <v>2.4511216859279399</v>
       </c>
     </row>
@@ -12285,23 +13399,23 @@
     </row>
     <row r="126" spans="1:19" s="83" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="85"/>
-      <c r="E126" s="119" t="s">
+      <c r="E126" s="124" t="s">
         <v>97</v>
       </c>
-      <c r="F126" s="119"/>
-      <c r="G126" s="119"/>
-      <c r="H126" s="119"/>
-      <c r="I126" s="119"/>
-      <c r="J126" s="119"/>
-      <c r="K126" s="119"/>
-      <c r="L126" s="119"/>
-      <c r="M126" s="119"/>
-      <c r="N126" s="119"/>
-      <c r="O126" s="119"/>
-      <c r="P126" s="119"/>
-      <c r="Q126" s="119"/>
-      <c r="R126" s="119"/>
-      <c r="S126" s="119"/>
+      <c r="F126" s="124"/>
+      <c r="G126" s="124"/>
+      <c r="H126" s="124"/>
+      <c r="I126" s="124"/>
+      <c r="J126" s="124"/>
+      <c r="K126" s="124"/>
+      <c r="L126" s="124"/>
+      <c r="M126" s="124"/>
+      <c r="N126" s="124"/>
+      <c r="O126" s="124"/>
+      <c r="P126" s="124"/>
+      <c r="Q126" s="124"/>
+      <c r="R126" s="124"/>
+      <c r="S126" s="124"/>
     </row>
     <row r="127" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B127" s="2" t="s">
@@ -14186,6 +15300,53 @@
       </c>
       <c r="S158" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="21" x14ac:dyDescent="0.65">
+      <c r="A162" s="64" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A163" t="s">
+        <v>320</v>
+      </c>
+      <c r="B163" t="s">
+        <v>321</v>
+      </c>
+      <c r="C163" t="s">
+        <v>322</v>
+      </c>
+      <c r="D163" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A164" t="s">
+        <v>21</v>
+      </c>
+      <c r="B164">
+        <v>153.88999999999999</v>
+      </c>
+      <c r="C164">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D164">
+        <v>127.36</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A165" t="s">
+        <v>185</v>
+      </c>
+      <c r="B165">
+        <v>440.44</v>
+      </c>
+      <c r="C165">
+        <v>30.95</v>
+      </c>
+      <c r="D165">
+        <v>395.79</v>
       </c>
     </row>
   </sheetData>
@@ -14203,6 +15364,1694 @@
     <mergeCell ref="O65:Q65"/>
     <mergeCell ref="J65:K65"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.53125" customWidth="1"/>
+    <col min="2" max="2" width="17.86328125" customWidth="1"/>
+    <col min="3" max="3" width="15.06640625" customWidth="1"/>
+    <col min="4" max="4" width="17.9296875" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.796875" customWidth="1"/>
+    <col min="7" max="7" width="16.53125" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" customWidth="1"/>
+    <col min="9" max="9" width="14.19921875" customWidth="1"/>
+    <col min="10" max="10" width="10.73046875" customWidth="1"/>
+    <col min="11" max="11" width="16.796875" customWidth="1"/>
+    <col min="13" max="13" width="15.19921875" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="64" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="83" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="126" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126" t="s">
+        <v>322</v>
+      </c>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" s="126"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>344</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>345</v>
+      </c>
+      <c r="F3" s="83" t="s">
+        <v>344</v>
+      </c>
+      <c r="G3" s="83" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.77555756156E-17</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.17792189894E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.0954451150100001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.1102230246299999E-16</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.41067359797E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1.44913767462E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="83" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.77555756156E-17</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9.6953597148299996E-3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6.7823299831300003E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="83" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.2555</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8.3754104376999997E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.1874342087E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1.2196310917699999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="83" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B8" s="50">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.4871191548299998E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F8" s="50">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.2884098726700001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="83" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="11" spans="1:15" s="83" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="1"/>
+      <c r="B11" s="126" t="s">
+        <v>375</v>
+      </c>
+      <c r="C11" s="126"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="131" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="131"/>
+      <c r="H11" s="131" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="131"/>
+      <c r="J11" s="131" t="s">
+        <v>370</v>
+      </c>
+      <c r="K11" s="131"/>
+      <c r="L11" s="131" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="131"/>
+      <c r="N11" s="131" t="s">
+        <v>371</v>
+      </c>
+      <c r="O11" s="131"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>372</v>
+      </c>
+      <c r="D12" t="s">
+        <v>373</v>
+      </c>
+      <c r="E12" t="s">
+        <v>374</v>
+      </c>
+      <c r="F12" s="108" t="s">
+        <v>369</v>
+      </c>
+      <c r="G12" s="108" t="s">
+        <v>367</v>
+      </c>
+      <c r="H12" s="108" t="s">
+        <v>369</v>
+      </c>
+      <c r="I12" s="108" t="s">
+        <v>367</v>
+      </c>
+      <c r="J12" s="108" t="s">
+        <v>369</v>
+      </c>
+      <c r="K12" s="108" t="s">
+        <v>367</v>
+      </c>
+      <c r="L12" s="108" t="s">
+        <v>369</v>
+      </c>
+      <c r="M12" s="108" t="s">
+        <v>367</v>
+      </c>
+      <c r="N12" s="108" t="s">
+        <v>369</v>
+      </c>
+      <c r="O12" s="108" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B13" s="1">
+        <f>H13/F13</f>
+        <v>2.5776288619628316</v>
+      </c>
+      <c r="C13" s="1">
+        <f>J13/F13</f>
+        <v>0.99064947208477816</v>
+      </c>
+      <c r="D13" s="1">
+        <f>(L13-J13)/F13</f>
+        <v>0.25119154296697443</v>
+      </c>
+      <c r="E13" s="1">
+        <f>(N13-J13)/F13</f>
+        <v>1.053194114362151</v>
+      </c>
+      <c r="F13" s="1">
+        <v>7.7001E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>10500</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.19847999999999999</v>
+      </c>
+      <c r="I13" s="1">
+        <v>10500</v>
+      </c>
+      <c r="J13" s="1">
+        <v>7.6281000000000002E-2</v>
+      </c>
+      <c r="K13" s="1">
+        <v>10500</v>
+      </c>
+      <c r="L13" s="1">
+        <v>9.5623E-2</v>
+      </c>
+      <c r="M13" s="1">
+        <v>10500</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0.15737799999999999</v>
+      </c>
+      <c r="O13" s="1">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" ref="B14:B33" si="0">H14/F14</f>
+        <v>2.284734737553503</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:C33" si="1">J14/F14</f>
+        <v>0.99753604415408859</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" ref="D14:D33" si="2">(L14-J14)/F14</f>
+        <v>0.1681403469249832</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" ref="E14:E33" si="3">(N14-J14)/F14</f>
+        <v>0.91825298490651042</v>
+      </c>
+      <c r="F14" s="1">
+        <v>7.1024000000000004E-2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>11504</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.162271</v>
+      </c>
+      <c r="I14" s="1">
+        <v>11504</v>
+      </c>
+      <c r="J14" s="1">
+        <v>7.0848999999999995E-2</v>
+      </c>
+      <c r="K14" s="1">
+        <v>11504</v>
+      </c>
+      <c r="L14" s="1">
+        <v>8.2791000000000003E-2</v>
+      </c>
+      <c r="M14" s="1">
+        <v>11504</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0.13606699999999999</v>
+      </c>
+      <c r="O14" s="1">
+        <v>11504</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>5.8467691431824651</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0128237973242242</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.11816111585539429</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="3"/>
+        <v>4.4406774836322231</v>
+      </c>
+      <c r="F15" s="1">
+        <v>7.0260000000000003E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>11616</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.41079399999999999</v>
+      </c>
+      <c r="I15" s="1">
+        <v>11616</v>
+      </c>
+      <c r="J15" s="1">
+        <v>7.1161000000000002E-2</v>
+      </c>
+      <c r="K15" s="1">
+        <v>11616</v>
+      </c>
+      <c r="L15" s="1">
+        <v>7.9463000000000006E-2</v>
+      </c>
+      <c r="M15" s="1">
+        <v>11616</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0.38316299999999998</v>
+      </c>
+      <c r="O15" s="1">
+        <v>11616</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6375134553283099</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0002392058366225</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.24979069489295538</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1158354263844037</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3.3444000000000002E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>10500</v>
+      </c>
+      <c r="H16" s="1">
+        <v>8.8208999999999996E-2</v>
+      </c>
+      <c r="I16" s="1">
+        <v>10500</v>
+      </c>
+      <c r="J16" s="1">
+        <v>3.3452000000000003E-2</v>
+      </c>
+      <c r="K16" s="1">
+        <v>10500</v>
+      </c>
+      <c r="L16" s="1">
+        <v>4.1806000000000003E-2</v>
+      </c>
+      <c r="M16" s="1">
+        <v>10500</v>
+      </c>
+      <c r="N16" s="1">
+        <v>7.077E-2</v>
+      </c>
+      <c r="O16" s="1">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5548582315364787</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0206769023870894</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.21388546452986668</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0769920430348539</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.7846000000000001E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>11503</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4.5594000000000003E-2</v>
+      </c>
+      <c r="I17" s="1">
+        <v>11503</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1.8214999999999999E-2</v>
+      </c>
+      <c r="K17" s="1">
+        <v>11503</v>
+      </c>
+      <c r="L17" s="1">
+        <v>2.2032E-2</v>
+      </c>
+      <c r="M17" s="1">
+        <v>11503</v>
+      </c>
+      <c r="N17" s="1">
+        <v>3.7435000000000003E-2</v>
+      </c>
+      <c r="O17" s="1">
+        <v>11503</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5523727475052049</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.98693373537224494</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.27058654605499316</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1819226075095124</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1.3929E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>11502</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3.5552E-2</v>
+      </c>
+      <c r="I18" s="1">
+        <v>11502</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1.3747000000000001E-2</v>
+      </c>
+      <c r="K18" s="1">
+        <v>11502</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1.7516E-2</v>
+      </c>
+      <c r="M18" s="1">
+        <v>11502</v>
+      </c>
+      <c r="N18" s="1">
+        <v>3.0210000000000001E-2</v>
+      </c>
+      <c r="O18" s="1">
+        <v>11502</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8334115438761143</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.86625997184420456</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.13467855466916936</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="3"/>
+        <v>0.56546222430783666</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2.1310000000000001E-3</v>
+      </c>
+      <c r="G19" s="1">
+        <v>584</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3.9069999999999999E-3</v>
+      </c>
+      <c r="I19" s="1">
+        <v>584</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1.846E-3</v>
+      </c>
+      <c r="K19" s="1">
+        <v>584</v>
+      </c>
+      <c r="L19" s="1">
+        <v>2.1329999999999999E-3</v>
+      </c>
+      <c r="M19" s="1">
+        <v>584</v>
+      </c>
+      <c r="N19" s="1">
+        <v>3.0509999999999999E-3</v>
+      </c>
+      <c r="O19" s="1">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4380403458213258</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.005763688760807</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.22190201729106623</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0489913544668588</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3.4699999999999998E-4</v>
+      </c>
+      <c r="G20" s="1">
+        <v>421</v>
+      </c>
+      <c r="H20" s="1">
+        <v>8.4599999999999996E-4</v>
+      </c>
+      <c r="I20" s="1">
+        <v>421</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3.4900000000000003E-4</v>
+      </c>
+      <c r="K20" s="1">
+        <v>421</v>
+      </c>
+      <c r="L20" s="1">
+        <v>4.26E-4</v>
+      </c>
+      <c r="M20" s="1">
+        <v>421</v>
+      </c>
+      <c r="N20" s="1">
+        <v>7.1299999999999998E-4</v>
+      </c>
+      <c r="O20" s="1">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>3.475352112676056</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.42957746478873238</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="2"/>
+        <v>2.8169014084507008E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="3"/>
+        <v>0.13028169014084504</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2.8400000000000002E-4</v>
+      </c>
+      <c r="G21" s="1">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1">
+        <v>9.8700000000000003E-4</v>
+      </c>
+      <c r="I21" s="1">
+        <v>6</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1.22E-4</v>
+      </c>
+      <c r="K21" s="1">
+        <v>6</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1.2999999999999999E-4</v>
+      </c>
+      <c r="M21" s="1">
+        <v>6</v>
+      </c>
+      <c r="N21" s="1">
+        <v>1.5899999999999999E-4</v>
+      </c>
+      <c r="O21" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>2.186666666666667</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4844444444444445</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="2"/>
+        <v>0.12444444444444458</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="3"/>
+        <v>0.50666666666666671</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2.2499999999999999E-4</v>
+      </c>
+      <c r="G22" s="1">
+        <v>100</v>
+      </c>
+      <c r="H22" s="1">
+        <v>4.9200000000000003E-4</v>
+      </c>
+      <c r="I22" s="1">
+        <v>100</v>
+      </c>
+      <c r="J22" s="1">
+        <v>3.3399999999999999E-4</v>
+      </c>
+      <c r="K22" s="1">
+        <v>100</v>
+      </c>
+      <c r="L22" s="1">
+        <v>3.6200000000000002E-4</v>
+      </c>
+      <c r="M22" s="1">
+        <v>100</v>
+      </c>
+      <c r="N22" s="1">
+        <v>4.4799999999999999E-4</v>
+      </c>
+      <c r="O22" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7037037037037037</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="2"/>
+        <v>0.29629629629629622</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1481481481481481</v>
+      </c>
+      <c r="F23" s="1">
+        <v>5.3999999999999998E-5</v>
+      </c>
+      <c r="G23" s="1">
+        <v>80</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1.46E-4</v>
+      </c>
+      <c r="I23" s="1">
+        <v>80</v>
+      </c>
+      <c r="J23" s="1">
+        <v>6.3E-5</v>
+      </c>
+      <c r="K23" s="1">
+        <v>80</v>
+      </c>
+      <c r="L23" s="1">
+        <v>7.8999999999999996E-5</v>
+      </c>
+      <c r="M23" s="1">
+        <v>80</v>
+      </c>
+      <c r="N23" s="1">
+        <v>1.25E-4</v>
+      </c>
+      <c r="O23" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="2"/>
+        <v>0.11111111111111117</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="3"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F24" s="1">
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="G24" s="1">
+        <v>8</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2.8E-5</v>
+      </c>
+      <c r="I24" s="1">
+        <v>8</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="K24" s="1">
+        <v>8</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1.4E-5</v>
+      </c>
+      <c r="M24" s="1">
+        <v>8</v>
+      </c>
+      <c r="N24" s="1">
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="O24" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="3"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="F25" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="G25" s="1">
+        <v>8</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="I25" s="1">
+        <v>8</v>
+      </c>
+      <c r="J25" s="1">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="K25" s="1">
+        <v>8</v>
+      </c>
+      <c r="L25" s="1">
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="M25" s="1">
+        <v>8</v>
+      </c>
+      <c r="N25" s="1">
+        <v>1.1E-5</v>
+      </c>
+      <c r="O25" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="2"/>
+        <v>0.19999999999999993</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="3"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="F26" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1.2E-5</v>
+      </c>
+      <c r="I26" s="1">
+        <v>2</v>
+      </c>
+      <c r="J26" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="K26" s="1">
+        <v>2</v>
+      </c>
+      <c r="L26" s="1">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="M26" s="1">
+        <v>2</v>
+      </c>
+      <c r="N26" s="1">
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="O26" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="2"/>
+        <v>0.25000000000000017</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="F27" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="O27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="F28" s="1">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="I28" s="1">
+        <v>2</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="K28" s="1">
+        <v>2</v>
+      </c>
+      <c r="L28" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="M28" s="1">
+        <v>2</v>
+      </c>
+      <c r="N28" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="O28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="M29" s="1">
+        <v>1</v>
+      </c>
+      <c r="N29" s="1">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="O29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="I30" s="1">
+        <v>2</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="K30" s="1">
+        <v>2</v>
+      </c>
+      <c r="L30" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M30" s="1">
+        <v>2</v>
+      </c>
+      <c r="N30" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="O30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1</v>
+      </c>
+      <c r="L31" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="O31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1</v>
+      </c>
+      <c r="H32" s="1">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1</v>
+      </c>
+      <c r="J32" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1</v>
+      </c>
+      <c r="L32" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="M32" s="1">
+        <v>1</v>
+      </c>
+      <c r="N32" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="O32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="K33" s="1">
+        <v>1</v>
+      </c>
+      <c r="L33" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M33" s="1">
+        <v>1</v>
+      </c>
+      <c r="N33" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="O33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="D34" s="48"/>
+    </row>
+    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.65">
+      <c r="A35" s="64" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="83" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+      <c r="A36" s="64"/>
+      <c r="B36" s="126" t="s">
+        <v>321</v>
+      </c>
+      <c r="C36" s="126"/>
+      <c r="D36" s="126" t="s">
+        <v>322</v>
+      </c>
+      <c r="E36" s="126"/>
+      <c r="F36" s="126" t="s">
+        <v>343</v>
+      </c>
+      <c r="G36" s="126"/>
+    </row>
+    <row r="37" spans="1:15" s="83" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+      <c r="A37" s="64"/>
+      <c r="B37" s="83" t="s">
+        <v>344</v>
+      </c>
+      <c r="C37" s="83" t="s">
+        <v>345</v>
+      </c>
+      <c r="D37" s="83" t="s">
+        <v>344</v>
+      </c>
+      <c r="E37" s="83" t="s">
+        <v>345</v>
+      </c>
+      <c r="F37" s="83" t="s">
+        <v>344</v>
+      </c>
+      <c r="G37" s="83" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A38" s="83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="1">
+        <v>70.042500000000004</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2.2994564575100001E-2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>59.902500000000003</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.209520285414</v>
+      </c>
+      <c r="F38" s="1">
+        <v>9.8469999999999995</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.20990712231799999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A39" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="1">
+        <v>84.484999999999999</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.26411171878599998</v>
+      </c>
+      <c r="D39" s="1">
+        <v>60.901499999999999</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.27468663964599999</v>
+      </c>
+      <c r="F39" s="1">
+        <v>23.148499999999999</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.27337291380099998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.65">
+      <c r="A42" s="64" t="s">
+        <v>377</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="23.19921875" customWidth="1"/>
+    <col min="5" max="5" width="18.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="92" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="110" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" s="109" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="109" t="s">
+        <v>339</v>
+      </c>
+      <c r="E2" s="112" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="B3" s="108">
+        <v>0.24166000000000001</v>
+      </c>
+      <c r="C3" s="108">
+        <v>0.24165</v>
+      </c>
+      <c r="D3" s="108">
+        <f>B3/C3</f>
+        <v>1.0000413821642873</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="B4" s="108">
+        <v>3.5954700000000002</v>
+      </c>
+      <c r="C4" s="108">
+        <v>3.6</v>
+      </c>
+      <c r="D4" s="108">
+        <f t="shared" ref="D4:D10" si="0">B4/C4</f>
+        <v>0.99874166666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="B5" s="108">
+        <v>1.048576</v>
+      </c>
+      <c r="C5" s="108">
+        <v>1.048576</v>
+      </c>
+      <c r="D5" s="108">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="16" t="s">
+        <v>329</v>
+      </c>
+      <c r="B6" s="108">
+        <v>20.561720000000001</v>
+      </c>
+      <c r="C6" s="108">
+        <v>19.753520000000002</v>
+      </c>
+      <c r="D6" s="108">
+        <f t="shared" si="0"/>
+        <v>1.0409142269327187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="B7" s="108">
+        <v>222.30833000000001</v>
+      </c>
+      <c r="C7" s="108">
+        <v>134.04006999999999</v>
+      </c>
+      <c r="D7" s="108">
+        <f t="shared" si="0"/>
+        <v>1.6585214406408475</v>
+      </c>
+      <c r="E7" s="1">
+        <v>138.51668000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="B8" s="108">
+        <v>211.57599999999999</v>
+      </c>
+      <c r="C8" s="108">
+        <v>123.88479</v>
+      </c>
+      <c r="D8" s="108">
+        <f t="shared" si="0"/>
+        <v>1.7078448451985107</v>
+      </c>
+      <c r="E8" s="1">
+        <v>127.87208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="111" t="s">
+        <v>331</v>
+      </c>
+      <c r="B9" s="108">
+        <v>1.09212</v>
+      </c>
+      <c r="C9" s="108">
+        <v>1.09426</v>
+      </c>
+      <c r="D9" s="108">
+        <f t="shared" si="0"/>
+        <v>0.99804434046753054</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="111" t="s">
+        <v>330</v>
+      </c>
+      <c r="B10" s="108">
+        <v>0.36</v>
+      </c>
+      <c r="C10" s="108">
+        <v>0.36055999999999999</v>
+      </c>
+      <c r="D10" s="108">
+        <f t="shared" si="0"/>
+        <v>0.99844686043931663</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="83"/>
+      <c r="B13" s="83" t="s">
+        <v>324</v>
+      </c>
+      <c r="C13" s="83" t="s">
+        <v>325</v>
+      </c>
+      <c r="D13" s="83" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B14" s="1">
+        <v>70487156332.800003</v>
+      </c>
+      <c r="C14" s="1">
+        <v>69571228782.399994</v>
+      </c>
+      <c r="D14" s="1">
+        <f>B14/C14</f>
+        <v>1.0131653208722931</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>334</v>
+      </c>
+      <c r="B15" s="1">
+        <v>287805360847</v>
+      </c>
+      <c r="C15" s="1">
+        <v>274726833509</v>
+      </c>
+      <c r="D15" s="1">
+        <f>B15/C15</f>
+        <v>1.0476055693976161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>335</v>
+      </c>
+      <c r="B16" s="1">
+        <v>53092433.600000001</v>
+      </c>
+      <c r="C16" s="1">
+        <v>50382460.799999997</v>
+      </c>
+      <c r="D16" s="1">
+        <f>B16/C16</f>
+        <v>1.0537880198181984</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="21" x14ac:dyDescent="0.65">
+      <c r="A20" s="92" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>341</v>
+      </c>
+      <c r="B21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -14238,11 +17087,11 @@
       <c r="D1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -14671,11 +17520,11 @@
       <c r="D20" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="108" t="s">
+      <c r="E20" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="108"/>
-      <c r="G20" s="108"/>
+      <c r="F20" s="113"/>
+      <c r="G20" s="113"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
@@ -15104,11 +17953,11 @@
       <c r="D39" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="108" t="s">
+      <c r="E39" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="108"/>
-      <c r="G39" s="108"/>
+      <c r="F39" s="113"/>
+      <c r="G39" s="113"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
@@ -15554,14 +18403,14 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="34"/>
-      <c r="B1" s="109" t="s">
+      <c r="B1" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="110"/>
-      <c r="D1" s="111" t="s">
+      <c r="C1" s="115"/>
+      <c r="D1" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="108"/>
+      <c r="E1" s="113"/>
     </row>
     <row r="2" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="34" t="s">
@@ -15888,14 +18737,14 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="34"/>
-      <c r="B21" s="109" t="s">
+      <c r="B21" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="110"/>
-      <c r="D21" s="111" t="s">
+      <c r="C21" s="115"/>
+      <c r="D21" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="108"/>
+      <c r="E21" s="113"/>
     </row>
     <row r="22" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="34" t="s">
@@ -16260,20 +19109,20 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7"/>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="115" t="s">
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
@@ -16871,20 +19720,20 @@
       </c>
     </row>
     <row r="19" spans="1:11" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="121" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="118"/>
-      <c r="G19" s="115" t="s">
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="123"/>
+      <c r="G19" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="115"/>
-      <c r="I19" s="115"/>
-      <c r="J19" s="115"/>
-      <c r="K19" s="115"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="120"/>
+      <c r="K19" s="120"/>
     </row>
     <row r="20" spans="1:11" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="8" t="s">
@@ -17532,8 +20381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S202"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17753,23 +20602,23 @@
       <c r="A15" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="119" t="s">
+      <c r="E15" s="124" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="119"/>
-      <c r="G15" s="119"/>
-      <c r="H15" s="119"/>
-      <c r="I15" s="119"/>
-      <c r="J15" s="119"/>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
-      <c r="M15" s="119"/>
-      <c r="N15" s="119"/>
-      <c r="O15" s="119"/>
-      <c r="P15" s="119"/>
-      <c r="Q15" s="119"/>
-      <c r="R15" s="119"/>
-      <c r="S15" s="119"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="124"/>
+      <c r="O15" s="124"/>
+      <c r="P15" s="124"/>
+      <c r="Q15" s="124"/>
+      <c r="R15" s="124"/>
+      <c r="S15" s="124"/>
     </row>
     <row r="16" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -18607,23 +21456,23 @@
       <c r="A32" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="119" t="s">
+      <c r="E32" s="124" t="s">
         <v>97</v>
       </c>
-      <c r="F32" s="119"/>
-      <c r="G32" s="119"/>
-      <c r="H32" s="119"/>
-      <c r="I32" s="119"/>
-      <c r="J32" s="119"/>
-      <c r="K32" s="119"/>
-      <c r="L32" s="119"/>
-      <c r="M32" s="119"/>
-      <c r="N32" s="119"/>
-      <c r="O32" s="119"/>
-      <c r="P32" s="119"/>
-      <c r="Q32" s="119"/>
-      <c r="R32" s="119"/>
-      <c r="S32" s="119"/>
+      <c r="F32" s="124"/>
+      <c r="G32" s="124"/>
+      <c r="H32" s="124"/>
+      <c r="I32" s="124"/>
+      <c r="J32" s="124"/>
+      <c r="K32" s="124"/>
+      <c r="L32" s="124"/>
+      <c r="M32" s="124"/>
+      <c r="N32" s="124"/>
+      <c r="O32" s="124"/>
+      <c r="P32" s="124"/>
+      <c r="Q32" s="124"/>
+      <c r="R32" s="124"/>
+      <c r="S32" s="124"/>
     </row>
     <row r="33" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
@@ -19633,23 +22482,23 @@
       <c r="A62" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="E62" s="119" t="s">
+      <c r="E62" s="124" t="s">
         <v>97</v>
       </c>
-      <c r="F62" s="119"/>
-      <c r="G62" s="119"/>
-      <c r="H62" s="119"/>
-      <c r="I62" s="119"/>
-      <c r="J62" s="119"/>
-      <c r="K62" s="119"/>
-      <c r="L62" s="119"/>
-      <c r="M62" s="119"/>
-      <c r="N62" s="119"/>
-      <c r="O62" s="119"/>
-      <c r="P62" s="119"/>
-      <c r="Q62" s="119"/>
-      <c r="R62" s="119"/>
-      <c r="S62" s="119"/>
+      <c r="F62" s="124"/>
+      <c r="G62" s="124"/>
+      <c r="H62" s="124"/>
+      <c r="I62" s="124"/>
+      <c r="J62" s="124"/>
+      <c r="K62" s="124"/>
+      <c r="L62" s="124"/>
+      <c r="M62" s="124"/>
+      <c r="N62" s="124"/>
+      <c r="O62" s="124"/>
+      <c r="P62" s="124"/>
+      <c r="Q62" s="124"/>
+      <c r="R62" s="124"/>
+      <c r="S62" s="124"/>
     </row>
     <row r="63" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
@@ -20484,23 +23333,23 @@
       <c r="A79" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="E79" s="119" t="s">
+      <c r="E79" s="124" t="s">
         <v>97</v>
       </c>
-      <c r="F79" s="119"/>
-      <c r="G79" s="119"/>
-      <c r="H79" s="119"/>
-      <c r="I79" s="119"/>
-      <c r="J79" s="119"/>
-      <c r="K79" s="119"/>
-      <c r="L79" s="119"/>
-      <c r="M79" s="119"/>
-      <c r="N79" s="119"/>
-      <c r="O79" s="119"/>
-      <c r="P79" s="119"/>
-      <c r="Q79" s="119"/>
-      <c r="R79" s="119"/>
-      <c r="S79" s="119"/>
+      <c r="F79" s="124"/>
+      <c r="G79" s="124"/>
+      <c r="H79" s="124"/>
+      <c r="I79" s="124"/>
+      <c r="J79" s="124"/>
+      <c r="K79" s="124"/>
+      <c r="L79" s="124"/>
+      <c r="M79" s="124"/>
+      <c r="N79" s="124"/>
+      <c r="O79" s="124"/>
+      <c r="P79" s="124"/>
+      <c r="Q79" s="124"/>
+      <c r="R79" s="124"/>
+      <c r="S79" s="124"/>
     </row>
     <row r="80" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
@@ -21697,23 +24546,23 @@
       <c r="A126" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="E126" s="119" t="s">
+      <c r="E126" s="124" t="s">
         <v>97</v>
       </c>
-      <c r="F126" s="119"/>
-      <c r="G126" s="119"/>
-      <c r="H126" s="119"/>
-      <c r="I126" s="119"/>
-      <c r="J126" s="119"/>
-      <c r="K126" s="119"/>
-      <c r="L126" s="119"/>
-      <c r="M126" s="119"/>
-      <c r="N126" s="119"/>
-      <c r="O126" s="119"/>
-      <c r="P126" s="119"/>
-      <c r="Q126" s="119"/>
-      <c r="R126" s="119"/>
-      <c r="S126" s="119"/>
+      <c r="F126" s="124"/>
+      <c r="G126" s="124"/>
+      <c r="H126" s="124"/>
+      <c r="I126" s="124"/>
+      <c r="J126" s="124"/>
+      <c r="K126" s="124"/>
+      <c r="L126" s="124"/>
+      <c r="M126" s="124"/>
+      <c r="N126" s="124"/>
+      <c r="O126" s="124"/>
+      <c r="P126" s="124"/>
+      <c r="Q126" s="124"/>
+      <c r="R126" s="124"/>
+      <c r="S126" s="124"/>
     </row>
     <row r="127" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
@@ -22492,23 +25341,23 @@
       <c r="A141" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="E141" s="119" t="s">
+      <c r="E141" s="124" t="s">
         <v>97</v>
       </c>
-      <c r="F141" s="119"/>
-      <c r="G141" s="119"/>
-      <c r="H141" s="119"/>
-      <c r="I141" s="119"/>
-      <c r="J141" s="119"/>
-      <c r="K141" s="119"/>
-      <c r="L141" s="119"/>
-      <c r="M141" s="119"/>
-      <c r="N141" s="119"/>
-      <c r="O141" s="119"/>
-      <c r="P141" s="119"/>
-      <c r="Q141" s="119"/>
-      <c r="R141" s="119"/>
-      <c r="S141" s="119"/>
+      <c r="F141" s="124"/>
+      <c r="G141" s="124"/>
+      <c r="H141" s="124"/>
+      <c r="I141" s="124"/>
+      <c r="J141" s="124"/>
+      <c r="K141" s="124"/>
+      <c r="L141" s="124"/>
+      <c r="M141" s="124"/>
+      <c r="N141" s="124"/>
+      <c r="O141" s="124"/>
+      <c r="P141" s="124"/>
+      <c r="Q141" s="124"/>
+      <c r="R141" s="124"/>
+      <c r="S141" s="124"/>
     </row>
     <row r="142" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
@@ -23626,23 +26475,23 @@
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
-      <c r="E167" s="120" t="s">
+      <c r="E167" s="125" t="s">
         <v>97</v>
       </c>
-      <c r="F167" s="120"/>
-      <c r="G167" s="120"/>
-      <c r="H167" s="120"/>
-      <c r="I167" s="120"/>
-      <c r="J167" s="120"/>
-      <c r="K167" s="120"/>
-      <c r="L167" s="120"/>
-      <c r="M167" s="120"/>
-      <c r="N167" s="120"/>
-      <c r="O167" s="120"/>
-      <c r="P167" s="120"/>
-      <c r="Q167" s="120"/>
-      <c r="R167" s="120"/>
-      <c r="S167" s="120"/>
+      <c r="F167" s="125"/>
+      <c r="G167" s="125"/>
+      <c r="H167" s="125"/>
+      <c r="I167" s="125"/>
+      <c r="J167" s="125"/>
+      <c r="K167" s="125"/>
+      <c r="L167" s="125"/>
+      <c r="M167" s="125"/>
+      <c r="N167" s="125"/>
+      <c r="O167" s="125"/>
+      <c r="P167" s="125"/>
+      <c r="Q167" s="125"/>
+      <c r="R167" s="125"/>
+      <c r="S167" s="125"/>
     </row>
     <row r="168" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A168" s="1" t="s">
@@ -24186,23 +27035,23 @@
       <c r="A186" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="E186" s="119" t="s">
+      <c r="E186" s="124" t="s">
         <v>97</v>
       </c>
-      <c r="F186" s="119"/>
-      <c r="G186" s="119"/>
-      <c r="H186" s="119"/>
-      <c r="I186" s="119"/>
-      <c r="J186" s="119"/>
-      <c r="K186" s="119"/>
-      <c r="L186" s="119"/>
-      <c r="M186" s="119"/>
-      <c r="N186" s="119"/>
-      <c r="O186" s="119"/>
-      <c r="P186" s="119"/>
-      <c r="Q186" s="119"/>
-      <c r="R186" s="119"/>
-      <c r="S186" s="119"/>
+      <c r="F186" s="124"/>
+      <c r="G186" s="124"/>
+      <c r="H186" s="124"/>
+      <c r="I186" s="124"/>
+      <c r="J186" s="124"/>
+      <c r="K186" s="124"/>
+      <c r="L186" s="124"/>
+      <c r="M186" s="124"/>
+      <c r="N186" s="124"/>
+      <c r="O186" s="124"/>
+      <c r="P186" s="124"/>
+      <c r="Q186" s="124"/>
+      <c r="R186" s="124"/>
+      <c r="S186" s="124"/>
     </row>
     <row r="187" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
@@ -24328,19 +27177,19 @@
       </c>
     </row>
     <row r="194" spans="1:4" s="83" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B194" s="119" t="s">
+      <c r="B194" s="124" t="s">
         <v>195</v>
       </c>
-      <c r="C194" s="119" t="s">
+      <c r="C194" s="124" t="s">
         <v>196</v>
       </c>
-      <c r="D194" s="119"/>
+      <c r="D194" s="124"/>
     </row>
     <row r="195" spans="1:4" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A195" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B195" s="119"/>
+      <c r="B195" s="124"/>
       <c r="C195" s="2" t="s">
         <v>185</v>
       </c>
@@ -24485,23 +27334,23 @@
       <c r="A2" s="84" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="126" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
       <c r="I2" s="74"/>
-      <c r="J2" s="121" t="s">
+      <c r="J2" s="126" t="s">
         <v>178</v>
       </c>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="126"/>
+      <c r="N2" s="126"/>
+      <c r="O2" s="126"/>
     </row>
     <row r="3" spans="1:17" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -24656,14 +27505,14 @@
       <c r="C7" s="83"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B8" s="121" t="s">
+      <c r="B8" s="126" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="121"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
     </row>
     <row r="9" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="83" t="s">
@@ -25042,23 +27891,23 @@
       <c r="A35" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="E35" s="119" t="s">
+      <c r="E35" s="124" t="s">
         <v>97</v>
       </c>
-      <c r="F35" s="119"/>
-      <c r="G35" s="119"/>
-      <c r="H35" s="119"/>
-      <c r="I35" s="119"/>
-      <c r="J35" s="119"/>
-      <c r="K35" s="119"/>
-      <c r="L35" s="119"/>
-      <c r="M35" s="119"/>
-      <c r="N35" s="119"/>
-      <c r="O35" s="119"/>
-      <c r="P35" s="119"/>
-      <c r="Q35" s="119"/>
-      <c r="R35" s="119"/>
-      <c r="S35" s="119"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="124"/>
+      <c r="H35" s="124"/>
+      <c r="I35" s="124"/>
+      <c r="J35" s="124"/>
+      <c r="K35" s="124"/>
+      <c r="L35" s="124"/>
+      <c r="M35" s="124"/>
+      <c r="N35" s="124"/>
+      <c r="O35" s="124"/>
+      <c r="P35" s="124"/>
+      <c r="Q35" s="124"/>
+      <c r="R35" s="124"/>
+      <c r="S35" s="124"/>
     </row>
     <row r="36" spans="1:19" s="83" customFormat="1" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
@@ -26905,23 +29754,23 @@
       <c r="B71" s="83"/>
       <c r="C71" s="83"/>
       <c r="D71" s="83"/>
-      <c r="E71" s="119" t="s">
+      <c r="E71" s="124" t="s">
         <v>97</v>
       </c>
-      <c r="F71" s="119"/>
-      <c r="G71" s="119"/>
-      <c r="H71" s="119"/>
-      <c r="I71" s="119"/>
-      <c r="J71" s="119"/>
-      <c r="K71" s="119"/>
-      <c r="L71" s="119"/>
-      <c r="M71" s="119"/>
-      <c r="N71" s="119"/>
-      <c r="O71" s="119"/>
-      <c r="P71" s="119"/>
-      <c r="Q71" s="119"/>
-      <c r="R71" s="119"/>
-      <c r="S71" s="119"/>
+      <c r="F71" s="124"/>
+      <c r="G71" s="124"/>
+      <c r="H71" s="124"/>
+      <c r="I71" s="124"/>
+      <c r="J71" s="124"/>
+      <c r="K71" s="124"/>
+      <c r="L71" s="124"/>
+      <c r="M71" s="124"/>
+      <c r="N71" s="124"/>
+      <c r="O71" s="124"/>
+      <c r="P71" s="124"/>
+      <c r="Q71" s="124"/>
+      <c r="R71" s="124"/>
+      <c r="S71" s="124"/>
     </row>
     <row r="72" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
@@ -32571,10 +35420,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView topLeftCell="C42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55:K64"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -32597,23 +35446,23 @@
       <c r="A1" s="79" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="127" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122" t="s">
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
-      <c r="L1" s="122"/>
-      <c r="M1" s="122"/>
-      <c r="N1" s="122"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="44"/>
@@ -33246,11 +36095,11 @@
       <c r="A25" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="128" t="s">
         <v>185</v>
       </c>
-      <c r="D25" s="123"/>
-      <c r="E25" s="123"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B26" s="40" t="s">
@@ -33473,14 +36322,14 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B40" s="121" t="s">
+      <c r="B40" s="126" t="s">
         <v>169</v>
       </c>
-      <c r="C40" s="121"/>
-      <c r="D40" s="121" t="s">
+      <c r="C40" s="126"/>
+      <c r="D40" s="126" t="s">
         <v>135</v>
       </c>
-      <c r="E40" s="121"/>
+      <c r="E40" s="126"/>
     </row>
     <row r="41" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B41" s="2" t="s">
@@ -33642,29 +36491,29 @@
       <c r="A55" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="B55" s="121" t="s">
+      <c r="B55" s="126" t="s">
         <v>274</v>
       </c>
-      <c r="C55" s="121"/>
-      <c r="D55" s="121" t="s">
+      <c r="C55" s="126"/>
+      <c r="D55" s="126" t="s">
         <v>275</v>
       </c>
-      <c r="E55" s="121"/>
-      <c r="F55" s="121"/>
-      <c r="G55" s="119" t="s">
+      <c r="E55" s="126"/>
+      <c r="F55" s="126"/>
+      <c r="G55" s="124" t="s">
         <v>280</v>
       </c>
-      <c r="H55" s="119"/>
-      <c r="I55" s="119"/>
-      <c r="J55" s="119" t="s">
+      <c r="H55" s="124"/>
+      <c r="I55" s="124"/>
+      <c r="J55" s="124" t="s">
         <v>285</v>
       </c>
-      <c r="K55" s="119"/>
-      <c r="L55" s="119" t="s">
+      <c r="K55" s="124"/>
+      <c r="L55" s="124" t="s">
         <v>292</v>
       </c>
-      <c r="M55" s="119"/>
-      <c r="N55" s="119"/>
+      <c r="M55" s="124"/>
+      <c r="N55" s="124"/>
     </row>
     <row r="56" spans="1:15" s="83" customFormat="1" ht="57.75" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="98"/>
@@ -34091,6 +36940,286 @@
         <v>0.99919865152394371</v>
       </c>
       <c r="O64" s="1"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A68" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="1">
+        <v>18.707609999999999</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0.34311779158200001</v>
+      </c>
+      <c r="D68" s="1">
+        <v>18.539439999999999</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0.494798812044</v>
+      </c>
+      <c r="F68" s="1">
+        <v>18.717590000000001</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0.48172959105699997</v>
+      </c>
+      <c r="H68" s="1">
+        <v>19.27383</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0.50217574025400002</v>
+      </c>
+      <c r="J68" s="1">
+        <v>19.311330000000002</v>
+      </c>
+      <c r="K68" s="1">
+        <v>0.40799420351299998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1.38777878078E-17</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0.17061000000000001</v>
+      </c>
+      <c r="E69" s="1">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0.19059999999999999</v>
+      </c>
+      <c r="G69" s="1">
+        <v>2.77555756156E-17</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0.22302</v>
+      </c>
+      <c r="I69" s="1">
+        <v>7.4833147735500001E-5</v>
+      </c>
+      <c r="J69" s="1">
+        <v>0.24218000000000001</v>
+      </c>
+      <c r="K69" s="1">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A70" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1.4974000000000001</v>
+      </c>
+      <c r="C70" s="1">
+        <v>5.7965506984799999E-4</v>
+      </c>
+      <c r="D70" s="1">
+        <v>1.6767099999999999</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1.81463494951E-3</v>
+      </c>
+      <c r="F70" s="1">
+        <v>2.06271</v>
+      </c>
+      <c r="G70" s="1">
+        <v>1.5062868252800001E-3</v>
+      </c>
+      <c r="H70" s="1">
+        <v>3.2185700000000002</v>
+      </c>
+      <c r="I70" s="1">
+        <v>8.4867013615400003E-3</v>
+      </c>
+      <c r="J70" s="1">
+        <v>3.6648999999999998</v>
+      </c>
+      <c r="K70" s="1">
+        <v>8.8081780181800007E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A71" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B71" s="1">
+        <v>56.549370000000003</v>
+      </c>
+      <c r="C71" s="1">
+        <v>6.7281008464499997E-2</v>
+      </c>
+      <c r="D71" s="1">
+        <v>109.04902</v>
+      </c>
+      <c r="E71" s="1">
+        <v>7.4020170224099999E-2</v>
+      </c>
+      <c r="F71" s="1">
+        <v>113.70416</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0.10856360532000001</v>
+      </c>
+      <c r="H71" s="1">
+        <v>138.85346999999999</v>
+      </c>
+      <c r="I71" s="1">
+        <v>8.3559452487400002E-2</v>
+      </c>
+      <c r="J71" s="1">
+        <v>137.39860999999999</v>
+      </c>
+      <c r="K71" s="1">
+        <v>6.9342489860099998E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="1">
+        <v>51.481810000000003</v>
+      </c>
+      <c r="C72" s="1">
+        <v>6.4964043131599994E-2</v>
+      </c>
+      <c r="D72" s="1">
+        <v>101.1439</v>
+      </c>
+      <c r="E72" s="1">
+        <v>8.6232835973300004E-2</v>
+      </c>
+      <c r="F72" s="1">
+        <v>105.48269999999999</v>
+      </c>
+      <c r="G72" s="1">
+        <v>8.9563541689700002E-2</v>
+      </c>
+      <c r="H72" s="1">
+        <v>128.76743999999999</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0.219160330352</v>
+      </c>
+      <c r="J72" s="1">
+        <v>126.50931</v>
+      </c>
+      <c r="K72" s="1">
+        <v>7.0113970790399993E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A73" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" s="1">
+        <v>1.048576</v>
+      </c>
+      <c r="C73" s="1">
+        <v>2.22044604925E-16</v>
+      </c>
+      <c r="D73" s="1">
+        <v>1.048576</v>
+      </c>
+      <c r="E73" s="1">
+        <v>2.22044604925E-16</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1.048576</v>
+      </c>
+      <c r="G73" s="1">
+        <v>2.22044604925E-16</v>
+      </c>
+      <c r="H73" s="1">
+        <v>1.048576</v>
+      </c>
+      <c r="I73" s="1">
+        <v>2.22044604925E-16</v>
+      </c>
+      <c r="J73" s="1">
+        <v>1.048576</v>
+      </c>
+      <c r="K73" s="1">
+        <v>2.22044604925E-16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1.10772</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1.4386104406699999E-3</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.71711000000000003</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1.1545128842900001E-3</v>
+      </c>
+      <c r="F74" s="1">
+        <v>0.81406999999999996</v>
+      </c>
+      <c r="G74" s="1">
+        <v>1.26885775405E-4</v>
+      </c>
+      <c r="H74" s="1">
+        <v>1.0240800000000001</v>
+      </c>
+      <c r="I74" s="1">
+        <v>3.2496153618500001E-4</v>
+      </c>
+      <c r="J74" s="1">
+        <v>1.0899399999999999</v>
+      </c>
+      <c r="K74" s="1">
+        <v>1.96580772203E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A75" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.14710000000000001</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.2525</v>
+      </c>
+      <c r="E75" s="1">
+        <v>3.0659419433500001E-4</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0.27933000000000002</v>
+      </c>
+      <c r="G75" s="1">
+        <v>4.5825756949600001E-5</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0.33624999999999999</v>
+      </c>
+      <c r="I75" s="1">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="J75" s="1">
+        <v>0.36042999999999997</v>
+      </c>
+      <c r="K75" s="1">
+        <v>4.5825756949600001E-5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -34115,8 +37244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S130"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -39521,7 +42650,10 @@
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
-      <c r="D130" s="1"/>
+      <c r="D130" s="1">
+        <f>SUM(D119:D129)</f>
+        <v>2600225223.3999996</v>
+      </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>

</xml_diff>